<commit_message>
Cambios al word y al excel
</commit_message>
<xml_diff>
--- a/Docs/ISIS1225 - Tablas de Datos Lab 7.xlsx
+++ b/Docs/ISIS1225 - Tablas de Datos Lab 7.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes.sharepoint.com/sites/ISIS1225/Documentos compartidos/General/202110/Laboratorios/Lab 07 - Colisiones/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1902876135bf28ab/Documents/EDA/Lab 7/ISIS1225-S08-G04/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="511" documentId="8_{A25BB2A9-7879-4ABF-A93E-5BD797619927}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5A6E5986-5D76-40E6-8BB6-4E7550720C79}"/>
+  <xr:revisionPtr revIDLastSave="515" documentId="8_{A25BB2A9-7879-4ABF-A93E-5BD797619927}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D56505B7-3573-44A7-9F25-DF4A9287AB50}"/>
   <bookViews>
-    <workbookView xWindow="-2127" yWindow="7073" windowWidth="4267" windowHeight="2354" tabRatio="767" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-8244" yWindow="3072" windowWidth="15360" windowHeight="7812" tabRatio="767" activeTab="1" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab7" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <r>
       <t>Factor de Carga</t>
@@ -65,6 +65,24 @@
   </si>
   <si>
     <t>Consumo de Datos [kB]</t>
+  </si>
+  <si>
+    <t>0.30</t>
+  </si>
+  <si>
+    <t>0.50</t>
+  </si>
+  <si>
+    <t>0.80</t>
+  </si>
+  <si>
+    <t>2.00</t>
+  </si>
+  <si>
+    <t>4.00</t>
+  </si>
+  <si>
+    <t>6.00</t>
   </si>
 </sst>
 </file>
@@ -97,15 +115,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -113,16 +137,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -131,114 +161,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <b val="0"/>
@@ -252,109 +197,6 @@
         <vertAlign val="baseline"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -408,7 +250,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -481,7 +323,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -496,11 +338,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos Lab7'!$A$8:$C$8</c:f>
+              <c:f>'Datos Lab7'!$A$1:$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Carga de Catálogo CHAINING</c:v>
+                  <c:v>Carga de Catálogo PROBING</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -568,7 +410,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -577,16 +419,16 @@
             <c:numRef>
               <c:f>'Datos Lab7'!$B$3:$B$5</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>1327229.7290000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>105</c:v>
+                  <c:v>1327216.557</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>115</c:v>
+                  <c:v>1327203.328</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -595,16 +437,16 @@
             <c:numRef>
               <c:f>'Datos Lab7'!$C$3:$C$5</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>45</c:v>
+                  <c:v>27501.332999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55</c:v>
+                  <c:v>25872.62</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>75</c:v>
+                  <c:v>25009.814999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -694,7 +536,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -703,16 +545,16 @@
             <c:numRef>
               <c:f>'Datos Lab7'!$B$10:$B$12</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>1327249.331</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>120</c:v>
+                  <c:v>1327249.17</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>140</c:v>
+                  <c:v>1327248.8759999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -721,16 +563,16 @@
             <c:numRef>
               <c:f>'Datos Lab7'!$C$10:$C$12</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>90</c:v>
+                  <c:v>26056.816999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>28826.078000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>110</c:v>
+                  <c:v>29637.399000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -835,11 +677,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -873,7 +715,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1833162896"/>
@@ -957,11 +799,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -995,7 +837,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="696671312"/>
@@ -1012,6 +854,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.23580845273648848"/>
+          <c:y val="0.92266565629711228"/>
+          <c:w val="0.54304772030886705"/>
+          <c:h val="6.5203541175477955E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1037,7 +889,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1074,7 +926,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1637,7 +1489,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{CA07E00A-1DDB-47A3-B681-B59870FF7EA9}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1648,7 +1500,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8661768" cy="6283739"/>
+    <xdr:ext cx="8660296" cy="6281530"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -1678,31 +1530,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A2:C5" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A2:C5" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A2:C5" xr:uid="{B245DDE7-54F2-4A7A-AC17-5CA17DD7B03F}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Factor de Carga (PROBING)" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Consumo de Datos [kB]" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="Tiempo de Ejecución [ms]" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Factor de Carga (PROBING)"/>
+    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Consumo de Datos [kB]"/>
+    <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="Tiempo de Ejecución [ms]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A9:C12" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A9:C12" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A9:C12" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Factor de Carga (CHAINING)" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Consumo de Datos [kB]" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="Tiempo de Ejecución [ms]" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Factor de Carga (CHAINING)"/>
+    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Consumo de Datos [kB]"/>
+    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="Tiempo de Ejecución [ms]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2000,25 +1852,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.64453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.05859375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.8203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.77734375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2029,47 +1881,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A3" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>100</v>
-      </c>
-      <c r="C3" s="2">
-        <v>45</v>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1327229.7290000001</v>
+      </c>
+      <c r="C3" s="5">
+        <v>27501.332999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A4" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="B4" s="2">
-        <v>105</v>
-      </c>
-      <c r="C4" s="2">
-        <v>55</v>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1327216.557</v>
+      </c>
+      <c r="C4" s="7">
+        <v>25872.62</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A5" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="B5" s="2">
-        <v>115</v>
-      </c>
-      <c r="C5" s="2">
-        <v>75</v>
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="9">
+        <v>1327203.328</v>
+      </c>
+      <c r="C5" s="9">
+        <v>25009.814999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -2080,40 +1932,40 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A10" s="2">
-        <v>2</v>
-      </c>
-      <c r="B10" s="2">
-        <v>100</v>
-      </c>
-      <c r="C10" s="2">
-        <v>90</v>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1327249.331</v>
+      </c>
+      <c r="C10" s="5">
+        <v>26056.816999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A11" s="2">
-        <v>4</v>
-      </c>
-      <c r="B11" s="2">
-        <v>120</v>
-      </c>
-      <c r="C11" s="2">
-        <v>100</v>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7">
+        <v>1327249.17</v>
+      </c>
+      <c r="C11" s="7">
+        <v>28826.078000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A12" s="2">
-        <v>6</v>
-      </c>
-      <c r="B12" s="2">
-        <v>140</v>
-      </c>
-      <c r="C12" s="2">
-        <v>110</v>
+    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="9">
+        <v>1327248.8759999999</v>
+      </c>
+      <c r="C12" s="9">
+        <v>29637.399000000001</v>
       </c>
     </row>
-    <row r="21" ht="14.7" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="21" ht="14.7" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
@@ -2128,6 +1980,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010023858CF01A2EF24688B692775F4C60A4" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="04b510ef1bc187d79b842c792d256c41">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="164883f8-7691-4ecf-b54a-664c0d0edefe" xmlns:ns3="85e30bcc-d76c-4413-8e4d-2dce22fb0743" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9049981c3eb1ee76226ec9e2f8ecd7b4" ns2:_="" ns3:_="">
     <xsd:import namespace="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
@@ -2338,36 +2205,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93C2AFC4-FCA8-4617-A6BD-EF7AAAEEB795}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
-    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2390,9 +2231,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93C2AFC4-FCA8-4617-A6BD-EF7AAAEEB795}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
+    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>